<commit_message>
Updated readme and team log
</commit_message>
<xml_diff>
--- a/docs/teamLog.xlsx
+++ b/docs/teamLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="19">
   <si>
     <t>Carter Chase</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Activity</t>
   </si>
   <si>
-    <t>Time Spent</t>
-  </si>
-  <si>
     <t>Individual Totals</t>
   </si>
   <si>
@@ -47,6 +44,33 @@
   </si>
   <si>
     <t>Team Total</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Talked with ECE Engineers</t>
+  </si>
+  <si>
+    <t>Read Chapters in Book</t>
+  </si>
+  <si>
+    <t>ECE End Semester Presentation</t>
+  </si>
+  <si>
+    <t>Senior Capstone Initial Meeting</t>
+  </si>
+  <si>
+    <t>Team Meeting</t>
+  </si>
+  <si>
+    <t>Studied python</t>
+  </si>
+  <si>
+    <t>Team Meeting with ECE Engineers</t>
+  </si>
+  <si>
+    <t>Dr. Kim Senior Capstone Lecture</t>
   </si>
 </sst>
 </file>
@@ -70,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -125,17 +149,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -170,30 +183,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,128 +555,426 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.125" customWidth="1"/>
-    <col min="4" max="4" width="9" style="2"/>
-    <col min="7" max="7" width="8.875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="9" style="2"/>
-    <col min="12" max="12" width="9" style="4"/>
+    <col min="1" max="1" width="10.625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="25.625" customWidth="1"/>
+    <col min="3" max="3" width="5.625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.625" customWidth="1"/>
+    <col min="6" max="6" width="5.625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.625" customWidth="1"/>
+    <col min="9" max="9" width="5.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.625" customWidth="1"/>
+    <col min="12" max="12" width="5.625" style="2" customWidth="1"/>
     <col min="14" max="14" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="N1" s="11" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="N1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="2">
+        <f>SUM(C3:C2000)</f>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>42482</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="14">
+        <v>4</v>
+      </c>
+      <c r="D3" s="10">
+        <v>42482</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="14">
+        <v>4</v>
+      </c>
+      <c r="G3" s="10">
+        <v>42482</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="14">
+        <v>4</v>
+      </c>
+      <c r="J3" s="10">
+        <v>42482</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="14">
+        <v>4</v>
+      </c>
+      <c r="M3" s="11"/>
+      <c r="N3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="12"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="O3" s="2">
+        <f>SUM(F3:F2000)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>42485</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D4" s="12">
+        <v>42485</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G4" s="12">
+        <v>42485</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J4" s="12">
+        <v>42485</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="2">
+        <f>SUM(I3:I2000)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>42513</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>42513</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G5" s="12">
+        <v>42513</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J5" s="12">
+        <v>42513</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="6">
+        <f>SUM(L3:L2000)</f>
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>42541</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
+        <v>42600</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="12">
+        <v>42600</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="12">
+        <v>42600</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>42598</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4">
-        <f>SUM(C3:C2000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O3" s="4">
-        <f>SUM(F3:F2000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N4" s="2" t="s">
+      <c r="D7" s="12">
+        <v>42605</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G7" s="12">
+        <v>42605</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J7" s="12">
+        <v>42605</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="4">
+        <f>SUM(O2:O5)</f>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>42600</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="12">
+        <v>42608</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2">
         <v>2</v>
       </c>
-      <c r="O4" s="4">
-        <f>SUM(I3:I2000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="O5" s="10">
-        <f>SUM(L3:L2000)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O7" s="7">
-        <f>SUM(O2:O5)</f>
-        <v>0</v>
+      <c r="G8" s="12">
+        <v>42608</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="12">
+        <v>42608</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="12">
+        <v>42600</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="12">
+        <v>42608</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="12">
+        <v>42608</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="12">
+        <v>42608</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>42605</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="12">
+        <v>42608</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
+        <v>42608</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Looked over docs and made two small changes. Added some time.
</commit_message>
<xml_diff>
--- a/docs/teamLog.xlsx
+++ b/docs/teamLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>Carter Chase</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Trevor Sietz</t>
   </si>
   <si>
-    <t>Ben Smit</t>
-  </si>
-  <si>
     <t>Team Total</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>Draft of proposal and presentation</t>
+  </si>
+  <si>
+    <t>Looked over Docs</t>
   </si>
 </sst>
 </file>
@@ -561,24 +561,24 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="25.625" customWidth="1"/>
-    <col min="3" max="3" width="5.625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.625" customWidth="1"/>
-    <col min="6" max="6" width="5.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.625" customWidth="1"/>
-    <col min="9" max="9" width="5.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.625" customWidth="1"/>
-    <col min="12" max="12" width="5.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="13.25" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="12" max="12" width="5.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -615,7 +615,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>4</v>
@@ -624,7 +624,7 @@
         <v>5</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>4</v>
@@ -633,7 +633,7 @@
         <v>5</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>4</v>
@@ -642,7 +642,7 @@
         <v>5</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>0</v>
@@ -657,7 +657,7 @@
         <v>42482</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="11">
         <v>4</v>
@@ -666,7 +666,7 @@
         <v>42482</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="11">
         <v>4</v>
@@ -675,7 +675,7 @@
         <v>42482</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="11">
         <v>4</v>
@@ -684,7 +684,7 @@
         <v>42482</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L3" s="11">
         <v>4</v>
@@ -703,7 +703,7 @@
         <v>42485</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2">
         <v>1.5</v>
@@ -712,7 +712,7 @@
         <v>42485</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2">
         <v>1.5</v>
@@ -721,7 +721,7 @@
         <v>42485</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="2">
         <v>1.5</v>
@@ -730,7 +730,7 @@
         <v>42485</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L4" s="2">
         <v>1.5</v>
@@ -748,7 +748,7 @@
         <v>42513</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2">
         <v>1.5</v>
@@ -757,7 +757,7 @@
         <v>42513</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2">
         <v>1.5</v>
@@ -766,7 +766,7 @@
         <v>42513</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="2">
         <v>1.5</v>
@@ -775,17 +775,17 @@
         <v>42513</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L5" s="2">
         <v>1.5</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O5" s="6">
         <f>SUM(L3:L2000)</f>
-        <v>13.5</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -793,7 +793,7 @@
         <v>42541</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -802,7 +802,7 @@
         <v>42600</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -811,7 +811,7 @@
         <v>42600</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="2">
         <v>1</v>
@@ -820,7 +820,7 @@
         <v>42600</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" s="2">
         <v>1</v>
@@ -831,7 +831,7 @@
         <v>42598</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>4</v>
@@ -840,7 +840,7 @@
         <v>42605</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="2">
         <v>1.5</v>
@@ -849,7 +849,7 @@
         <v>42605</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I7" s="2">
         <v>1.5</v>
@@ -858,17 +858,17 @@
         <v>42605</v>
       </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L7" s="2">
         <v>1.5</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O7" s="4">
         <f>SUM(O2:O5)</f>
-        <v>66.5</v>
+        <v>66.75</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -876,7 +876,7 @@
         <v>42600</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2">
         <v>3</v>
@@ -885,7 +885,7 @@
         <v>42608</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2">
         <v>2</v>
@@ -894,7 +894,7 @@
         <v>42608</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I8" s="2">
         <v>2</v>
@@ -903,7 +903,7 @@
         <v>42608</v>
       </c>
       <c r="K8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L8" s="2">
         <v>2</v>
@@ -914,7 +914,7 @@
         <v>42600</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -923,7 +923,7 @@
         <v>42608</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="2">
         <v>2</v>
@@ -932,7 +932,7 @@
         <v>42608</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I9" s="2">
         <v>2</v>
@@ -941,7 +941,7 @@
         <v>42608</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L9" s="2">
         <v>2</v>
@@ -952,10 +952,19 @@
         <v>42605</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>1.5</v>
+      </c>
+      <c r="J10" s="9">
+        <v>42608</v>
+      </c>
+      <c r="K10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -963,7 +972,7 @@
         <v>42608</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -974,7 +983,7 @@
         <v>42608</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -985,7 +994,7 @@
         <v>42609</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2">
         <v>4.5</v>

</xml_diff>